<commit_message>
add current shunt and mosfet driven
</commit_message>
<xml_diff>
--- a/Project/Project managment sheet.xlsx
+++ b/Project/Project managment sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Embedded sytems programming project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Embedded Project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EDE587-E547-4BEE-8094-2B04AA218993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,9 +310,6 @@
     <t>Debugging</t>
   </si>
   <si>
-    <t>Testing the program. Also we  recieved our pcb from OSH Park.</t>
-  </si>
-  <si>
     <t xml:space="preserve">OVERVIEW: We recieved the pcb from OSH Park, and we are now testing how to read the cell voltages through the multiplexer. </t>
   </si>
   <si>
@@ -343,9 +341,6 @@
   </si>
   <si>
     <t>Did a new version on the copperboard.</t>
-  </si>
-  <si>
-    <t>Designing a circuit to add the temperature sensor so we can chack the cell temperatures.</t>
   </si>
   <si>
     <t>Looking into the shunt resistor to read the current coming out from the battery.</t>
@@ -443,12 +438,18 @@
   </si>
   <si>
     <t>Not able to get the data to the db.</t>
+  </si>
+  <si>
+    <t>Add the temperature sensor so we can chack the cell temperatures.</t>
+  </si>
+  <si>
+    <t>Design and testing temperature circuit  on breadboard with program. Also we  recieved our pcb from OSH Park.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -489,10 +490,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -500,6 +501,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="112">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1168,26 +1189,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1202,224 +1203,224 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 1 28.8.-1.9." dataDxfId="111"/>
-    <tableColumn id="2" name="Role" dataDxfId="110"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="109"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="108"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint 1 28.8.-1.9." dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Role" dataDxfId="108"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="what I did?" dataDxfId="107"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="What am I doing?" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Blockers" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14511" displayName="Table14511" ref="A40:E44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A40:E44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14511" displayName="Table14511" ref="A40:E44" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A40:E44" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 10 30.10.-3.11." dataDxfId="48"/>
-    <tableColumn id="2" name="Role" dataDxfId="47"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="46"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="45"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Sprint 10 30.10.-3.11." dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Role" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="what I did?" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="What am I doing?" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Blockers" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1451112" displayName="Table1451112" ref="A45:E48" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A45:E48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table1451112" displayName="Table1451112" ref="A45:E48" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A45:E48" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 11 6.11.-10.11." dataDxfId="41"/>
-    <tableColumn id="2" name="Role" dataDxfId="40"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="39"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="38"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Sprint 11 6.11.-10.11." dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Role" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="what I did?" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="What am I doing?" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Blockers" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1451113" displayName="Table1451113" ref="A49:E52" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A49:E52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table1451113" displayName="Table1451113" ref="A49:E52" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A49:E52" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 12 13.11.- 17.11." dataDxfId="34"/>
-    <tableColumn id="2" name="Role" dataDxfId="33"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="32"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="31"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Sprint 12 13.11.- 17.11." dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Role" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="what I did?" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="What am I doing?" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Blockers" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1451114" displayName="Table1451114" ref="A53:E57" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A53:E57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table1451114" displayName="Table1451114" ref="A53:E57" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A53:E57" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 13 20.11.- 24.11." dataDxfId="27"/>
-    <tableColumn id="2" name="Role" dataDxfId="26"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="25"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="24"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Sprint 13 20.11.- 24.11." dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Role" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="what I did?" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="What am I doing?" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Blockers" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1451115" displayName="Table1451115" ref="A58:E61" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A58:E61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table1451115" displayName="Table1451115" ref="A58:E61" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A58:E61" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 14 27.11.-1.12." dataDxfId="20"/>
-    <tableColumn id="2" name="Role" dataDxfId="19"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="18"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="17"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Sprint 14 27.11.-1.12." dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Role" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="what I did?" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="What am I doing?" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Blockers" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table145111516" displayName="Table145111516" ref="A62:E65" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A62:E65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table145111516" displayName="Table145111516" ref="A62:E65" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A62:E65" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 15 4.12.-8.12." dataDxfId="13"/>
-    <tableColumn id="2" name="Role" dataDxfId="12"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="11"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="10"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Sprint 15 4.12.-8.12." dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Role" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="what I did?" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="What am I doing?" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Blockers" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table145111517" displayName="Table145111517" ref="A66:E69" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A66:E69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table145111517" displayName="Table145111517" ref="A66:E69" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A66:E69" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 16 11.12.-15.12." dataDxfId="6"/>
-    <tableColumn id="2" name="Role" dataDxfId="5"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="4"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="3"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Sprint 16 11.12.-15.12." dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Role" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="what I did?" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="What am I doing?" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Blockers" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:E9" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
-  <autoFilter ref="A5:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A5:E9" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103">
+  <autoFilter ref="A5:E9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 2 4.9.-8.9" dataDxfId="104"/>
-    <tableColumn id="2" name="Role" dataDxfId="103"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="102"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="101"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Sprint 2 4.9.-8.9" dataDxfId="102"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Role" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="what I did?" dataDxfId="100"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="What am I doing?" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Blockers" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A10:E14" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
-  <autoFilter ref="A10:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:E14" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A10:E14" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 3 11.9.-15.9." dataDxfId="97"/>
-    <tableColumn id="2" name="Role" dataDxfId="96"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="95"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="94"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Sprint 3 11.9.-15.9." dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Role" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="what I did?" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="What am I doing?" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Blockers" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A15:E18" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
-  <autoFilter ref="A15:E18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table145" displayName="Table145" ref="A15:E18" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
+  <autoFilter ref="A15:E18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 4 18.9.-22.9." dataDxfId="90"/>
-    <tableColumn id="2" name="Role" dataDxfId="89"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="88"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="87"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sprint 4 18.9.-22.9." dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Role" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="what I did?" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="What am I doing?" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Blockers" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A19:E22" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
-  <autoFilter ref="A19:E22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1456" displayName="Table1456" ref="A19:E22" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A19:E22" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 5 25.9.-29.9." dataDxfId="83"/>
-    <tableColumn id="2" name="Role" dataDxfId="82"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="81"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="80"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Sprint 5 25.9.-29.9." dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Role" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="what I did?" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="What am I doing?" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Blockers" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1457" displayName="Table1457" ref="A23:E26" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="A23:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table1457" displayName="Table1457" ref="A23:E26" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+  <autoFilter ref="A23:E26" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 6 2.10.-6.10." dataDxfId="76"/>
-    <tableColumn id="2" name="Role" dataDxfId="75"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="74"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="73"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Sprint 6 2.10.-6.10." dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Role" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="what I did?" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="What am I doing?" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Blockers" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1458" displayName="Table1458" ref="A27:E31" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
-  <autoFilter ref="A27:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table1458" displayName="Table1458" ref="A27:E31" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+  <autoFilter ref="A27:E31" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 7 9.10.-13.10." dataDxfId="69"/>
-    <tableColumn id="2" name="Role" dataDxfId="68"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="67"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="66"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Sprint 7 9.10.-13.10." dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Role" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="what I did?" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="What am I doing?" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Blockers" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1459" displayName="Table1459" ref="A32:E35" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <autoFilter ref="A32:E35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table1459" displayName="Table1459" ref="A32:E35" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+  <autoFilter ref="A32:E35" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 8 16.10-20.10." dataDxfId="62"/>
-    <tableColumn id="2" name="Role" dataDxfId="61"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="60"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="59"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Sprint 8 16.10-20.10." dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Role" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="what I did?" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="What am I doing?" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Blockers" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table14510" displayName="Table14510" ref="A36:E39" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
-  <autoFilter ref="A36:E39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table14510" displayName="Table14510" ref="A36:E39" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A36:E39" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sprint 9 23.10.-27.10." dataDxfId="55"/>
-    <tableColumn id="2" name="Role" dataDxfId="54"/>
-    <tableColumn id="3" name="what I did?" dataDxfId="53"/>
-    <tableColumn id="4" name="What am I doing?" dataDxfId="52"/>
-    <tableColumn id="5" name="Blockers" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Sprint 9 23.10.-27.10." dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Role" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="what I did?" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="What am I doing?" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Blockers" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1687,23 +1688,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="50.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,7 +1815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1857,7 +1858,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1908,7 +1909,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1934,7 +1935,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2036,7 +2037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>73</v>
       </c>
@@ -2215,7 +2216,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -2332,7 +2333,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
@@ -2347,7 +2348,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>26</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2381,7 +2382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>1</v>
       </c>
@@ -2392,13 +2393,13 @@
         <v>91</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>2</v>
       </c>
@@ -2415,16 +2416,16 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>27</v>
       </c>
@@ -2441,7 +2442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2449,16 +2450,16 @@
         <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
@@ -2466,16 +2467,16 @@
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>2</v>
       </c>
@@ -2483,16 +2484,16 @@
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>28</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -2517,16 +2518,16 @@
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
@@ -2534,16 +2535,16 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
@@ -2551,16 +2552,16 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>29</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -2585,16 +2586,16 @@
         <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
@@ -2602,16 +2603,16 @@
         <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
@@ -2619,25 +2620,25 @@
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>30</v>
       </c>
@@ -2654,7 +2655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -2662,16 +2663,16 @@
         <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>1</v>
       </c>
@@ -2679,16 +2680,16 @@
         <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
@@ -2696,18 +2697,18 @@
         <v>4</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A62" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>3</v>
@@ -2722,7 +2723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -2730,16 +2731,16 @@
         <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>1</v>
       </c>
@@ -2747,16 +2748,16 @@
         <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>2</v>
       </c>
@@ -2764,18 +2765,18 @@
         <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A66" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>3</v>
@@ -2790,33 +2791,33 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D67" s="1" t="s">
+    </row>
+    <row r="68" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2825,7 +2826,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B6:B9 B11:B14 B16:B18 B20:B22 B24:B26 B28:B31 B33:B35 B37:B39 B41:B44 B46:B48 B50:B52 B54:B57 B59:B61 B63:B65 B67:B69">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B6:B9 B11:B14 B16:B18 B20:B22 B24:B26 B28:B31 B33:B35 B37:B39 B41:B44 B46:B48 B50:B52 B54:B57 B59:B61 B63:B65 B67:B69" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$Z$2:$Z$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>